<commit_message>
Update memorymap with RTC_old
</commit_message>
<xml_diff>
--- a/FSW/memorymap.xlsx
+++ b/FSW/memorymap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\CANSAT_2021\FSW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{84EA4D73-9B2E-400A-B48B-0518321AA781}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8ED63A42-CD25-4008-AA0E-E5CE125D9C64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12960" yWindow="1032" windowWidth="21600" windowHeight="11328"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="50">
   <si>
     <t>Shared</t>
   </si>
@@ -162,6 +162,15 @@
   </si>
   <si>
     <t>end_transmission_hh</t>
+  </si>
+  <si>
+    <t>mission_time_ss</t>
+  </si>
+  <si>
+    <t>mission_time_mm</t>
+  </si>
+  <si>
+    <t>mission_time_hh</t>
   </si>
 </sst>
 </file>
@@ -1090,8 +1099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1250,15 +1259,51 @@
       <c r="A10">
         <v>8</v>
       </c>
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Color code finished vars
</commit_message>
<xml_diff>
--- a/FSW/memorymap.xlsx
+++ b/FSW/memorymap.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\CANSAT_2021\FSW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8ED63A42-CD25-4008-AA0E-E5CE125D9C64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B373CC-97AA-4F9E-B5E7-D7AC0D9812BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12960" yWindow="1032" windowWidth="21600" windowHeight="11328"/>
+    <workbookView xWindow="-17540" yWindow="-1700" windowWidth="21600" windowHeight="11330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="memorymap" sheetId="1" r:id="rId1"/>
@@ -176,8 +176,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -320,8 +320,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -499,6 +507,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -724,7 +738,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -739,7 +753,9 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1096,11 +1112,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1140,7 +1156,7 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
@@ -1163,7 +1179,7 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E3" t="s">
@@ -1184,7 +1200,7 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E4" t="s">
@@ -1207,7 +1223,7 @@
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E5" t="s">
@@ -1224,7 +1240,7 @@
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E6" t="s">
@@ -1241,68 +1257,68 @@
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="10"/>
+      <c r="B7" s="12"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="10"/>
+      <c r="B8" s="12"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="10"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="B9" s="12"/>
+    </row>
+    <row r="10" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11">
+    <row r="11" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12">
+    <row r="12" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="10" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1375,7 +1391,7 @@
       <c r="A26">
         <v>24</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="11" t="s">
         <v>26</v>
       </c>
       <c r="E26" t="s">
@@ -1392,7 +1408,7 @@
       <c r="A27">
         <v>25</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="11" t="s">
         <v>41</v>
       </c>
       <c r="E27" t="s">
@@ -1409,7 +1425,7 @@
       <c r="A28">
         <v>26</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="12" t="s">
         <v>37</v>
       </c>
       <c r="E28" t="s">
@@ -1426,25 +1442,25 @@
       <c r="A29">
         <v>27</v>
       </c>
-      <c r="C29" s="10"/>
+      <c r="C29" s="12"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
-      <c r="C30" s="10"/>
+      <c r="C30" s="12"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
-      <c r="C31" s="10"/>
+      <c r="C31" s="12"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="11" t="s">
         <v>28</v>
       </c>
       <c r="E32" t="s">
@@ -1461,7 +1477,7 @@
       <c r="A33">
         <v>31</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="11" t="s">
         <v>29</v>
       </c>
       <c r="E33" t="s">
@@ -1478,7 +1494,7 @@
       <c r="A34">
         <v>32</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="12" t="s">
         <v>42</v>
       </c>
       <c r="E34" t="s">
@@ -1495,25 +1511,25 @@
       <c r="A35">
         <v>33</v>
       </c>
-      <c r="C35" s="10"/>
+      <c r="C35" s="12"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
-      <c r="C36" s="10"/>
+      <c r="C36" s="12"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
-      <c r="C37" s="10"/>
+      <c r="C37" s="12"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C38" s="12" t="s">
         <v>43</v>
       </c>
       <c r="E38" t="s">
@@ -1530,19 +1546,19 @@
       <c r="A39">
         <v>37</v>
       </c>
-      <c r="C39" s="10"/>
+      <c r="C39" s="12"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
-      <c r="C40" s="10"/>
+      <c r="C40" s="12"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
-      <c r="C41" s="10"/>
+      <c r="C41" s="12"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42">
@@ -1898,7 +1914,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>